<commit_message>
added total hours for time management
</commit_message>
<xml_diff>
--- a/work/Zeitmanagement.xlsx
+++ b/work/Zeitmanagement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis Sentler\Desktop\ESE\SEP\SE2-Projekt\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis Sentler\Desktop\ESE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1BDFCF-0425-43AB-9D25-23A910E4DD3A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E66B130A-4E5B-4AFE-8E52-1A666FF5F2F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agdas" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="Sentler" sheetId="3" r:id="rId3"/>
     <sheet name="Brak" sheetId="4" r:id="rId4"/>
     <sheet name="Kessener" sheetId="5" r:id="rId5"/>
+    <sheet name="Total" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Kessener!$A$1:$Z$7</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Datum</t>
   </si>
@@ -90,6 +91,12 @@
   </si>
   <si>
     <t>Selbstkalibrierung, FSM</t>
+  </si>
+  <si>
+    <t>Geplante Zeit:</t>
+  </si>
+  <si>
+    <t>Tatsächsliche Zeit:</t>
   </si>
 </sst>
 </file>
@@ -133,12 +140,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -455,11 +468,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,11 +495,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,15 +523,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43181</v>
       </c>
@@ -546,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43186</v>
       </c>
@@ -560,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43187</v>
       </c>
@@ -587,12 +600,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43184</v>
       </c>
@@ -620,7 +633,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43186</v>
       </c>
@@ -647,13 +660,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -681,7 +694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -695,7 +708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -709,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -723,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -737,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -755,4 +768,44 @@
   <autoFilter ref="A1:Z7" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F419C51-4153-4D2D-AB72-2EF46513CD85}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1">
+        <f>SUM(Agdas!C2:C100,Hussein!C2:C100,Sentler!C2:C100,Brak!C2:C100,Kessener!C2:C100)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="2">
+        <f>SUM(Agdas!D2:D100,Hussein!D2:D100,Sentler!D2:D100,Brak!D2:D100,Kessener!D2:D100)</f>
+        <v>21.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>